<commit_message>
Reorder microhum 16S rRNA datasets
</commit_message>
<xml_diff>
--- a/inst/extdata/microhum/SI/Table_S2.xlsx
+++ b/inst/extdata/microhum/SI/Table_S2.xlsx
@@ -98,16 +98,28 @@
     <t xml:space="preserve">PRJNA714242</t>
   </si>
   <si>
+    <t xml:space="preserve">VCV+21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA673585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSC+22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA777915</t>
+  </si>
+  <si>
     <t xml:space="preserve">HMH+21</t>
   </si>
   <si>
     <t xml:space="preserve">PRJNA726205</t>
   </si>
   <si>
-    <t xml:space="preserve">VCV+21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA673585</t>
+    <t xml:space="preserve">GKJ+22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA707350</t>
   </si>
   <si>
     <t xml:space="preserve">SRS+22</t>
@@ -116,18 +128,6 @@
     <t xml:space="preserve">PRJNA726992 PRJNA726994</t>
   </si>
   <si>
-    <t xml:space="preserve">CSC+22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA777915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GKJ+22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA707350</t>
-  </si>
-  <si>
     <t xml:space="preserve">HMA+22</t>
   </si>
   <si>
@@ -158,6 +158,12 @@
     <t xml:space="preserve">PRJNA780671</t>
   </si>
   <si>
+    <t xml:space="preserve">MAC+21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA669421</t>
+  </si>
+  <si>
     <t xml:space="preserve">XLZ+21</t>
   </si>
   <si>
@@ -167,12 +173,6 @@
     <t xml:space="preserve">(i)</t>
   </si>
   <si>
-    <t xml:space="preserve">MAC+21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA669421</t>
-  </si>
-  <si>
     <t xml:space="preserve">GWL+21</t>
   </si>
   <si>
@@ -233,6 +233,12 @@
     <t xml:space="preserve">PRJNA678695</t>
   </si>
   <si>
+    <t xml:space="preserve">MIK+22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJDB11949 PRJDB12349</t>
+  </si>
+  <si>
     <t xml:space="preserve">RDM+22</t>
   </si>
   <si>
@@ -242,12 +248,6 @@
     <t xml:space="preserve">(h)</t>
   </si>
   <si>
-    <t xml:space="preserve">MIK+22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJDB11949 PRJDB12349</t>
-  </si>
-  <si>
     <t xml:space="preserve">WZL+23</t>
   </si>
   <si>
@@ -260,6 +260,12 @@
     <t xml:space="preserve">PRJNA769052</t>
   </si>
   <si>
+    <t xml:space="preserve">GCP+23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJEB61723 PRJEB61722</t>
+  </si>
+  <si>
     <t xml:space="preserve">FBD+22</t>
   </si>
   <si>
@@ -272,12 +278,6 @@
     <t xml:space="preserve">PRJNA756849</t>
   </si>
   <si>
-    <t xml:space="preserve">GCP+23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJEB61723 PRJEB61722</t>
-  </si>
-  <si>
     <t xml:space="preserve">IBD gut</t>
   </si>
   <si>
@@ -308,52 +308,52 @@
     <t xml:space="preserve">(f)</t>
   </si>
   <si>
+    <t xml:space="preserve">LZD+19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA391149 (k)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLL+16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA313074</t>
+  </si>
+  <si>
     <t xml:space="preserve">PYL+23</t>
   </si>
   <si>
     <t xml:space="preserve">PRJNA975689</t>
   </si>
   <si>
-    <t xml:space="preserve">MLL+16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA313074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LZD+19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA391149 (k)</t>
-  </si>
-  <si>
     <t xml:space="preserve">BKK+17</t>
   </si>
   <si>
     <t xml:space="preserve">PRJNA368966</t>
   </si>
   <si>
+    <t xml:space="preserve">REP+23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJEB47161 PRJEB47162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAA+19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJNA398089 (j)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBL+17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJEB18471</t>
+  </si>
+  <si>
     <t xml:space="preserve">MDV+22</t>
   </si>
   <si>
     <t xml:space="preserve">PRJEB42155 (j)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAA+19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJNA398089 (j)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REP+23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJEB47161 PRJEB47162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBL+17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRJEB18471</t>
   </si>
   <si>
     <t xml:space="preserve">GKD+14</t>
@@ -667,9 +667,9 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K65" activeCellId="0" sqref="K65"/>
+      <selection pane="bottomLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -893,25 +893,25 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>104682</v>
+        <v>83816</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>37669</v>
+        <v>62283</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>54.9</v>
+        <v>16.8</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>5.7</v>
+        <v>2.7</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>5811</v>
+        <v>9687</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>99</v>
@@ -925,28 +925,28 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>83816</v>
+        <v>110953</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>62283</v>
+        <v>45756</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>16.8</v>
+        <v>48.5</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>2.7</v>
+        <v>3.5</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>9687</v>
+        <v>9556</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,28 +957,28 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>37360</v>
+        <v>104682</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>29921</v>
+        <v>37669</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>16</v>
+        <v>54.9</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0.6</v>
+        <v>5.7</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>5886</v>
+        <v>5811</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,28 +989,28 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>110953</v>
+        <v>112174</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>45756</v>
+        <v>88209</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>440</v>
+        <v>290</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>48.5</v>
+        <v>25.4</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>9556</v>
+        <v>9732</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,28 +1021,28 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>37360</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>29921</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>5886</v>
+      </c>
+      <c r="K17" s="1" t="n">
         <v>89</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>112174</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>88209</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>290</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <v>9732</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,7 +1073,7 @@
       <c r="J18" s="1" t="n">
         <v>9097</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>97</v>
       </c>
     </row>
@@ -1199,70 +1199,70 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>52638</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>32414</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>9528</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D27" s="1" t="n">
         <v>105509</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E27" s="1" t="n">
         <v>89883</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F27" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="2" t="n">
+      <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="2" t="n">
         <v>5.1</v>
       </c>
-      <c r="I26" s="2" t="n">
+      <c r="I27" s="2" t="n">
         <v>9.2</v>
       </c>
-      <c r="J26" s="1" t="n">
+      <c r="J27" s="1" t="n">
         <v>7772</v>
       </c>
-      <c r="K26" s="1" t="n">
+      <c r="K27" s="1" t="n">
         <v>94</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>52638</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>32414</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>350</v>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>9.8</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="J27" s="1" t="n">
-        <v>9528</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,63 +1586,63 @@
         <v>71</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>132</v>
+        <v>214</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>98023</v>
+        <v>123490</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>68904</v>
+        <v>79703</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>440</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H41" s="2" t="n">
-        <v>70.4</v>
+        <v>19.3</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>4633</v>
+        <v>9549</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="C42" s="1" t="n">
-        <v>214</v>
+        <v>132</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>123490</v>
+        <v>98023</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>79703</v>
+        <v>68904</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>440</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="H42" s="2" t="n">
-        <v>19.3</v>
+        <v>70.4</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="J42" s="1" t="n">
-        <v>9549</v>
+        <v>4633</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,31 +1717,28 @@
         <v>80</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>219</v>
+        <v>138</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>73309</v>
+        <v>255886</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>62137</v>
+        <v>180138</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>305</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>15</v>
+        <v>440</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>35.9</v>
+        <v>20.2</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>7.9</v>
+        <v>3.4</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>7218</v>
+        <v>9655</v>
       </c>
       <c r="K45" s="1" t="n">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,28 +1749,31 @@
         <v>82</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>29353</v>
+        <v>73309</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>20421</v>
+        <v>62137</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>440</v>
+        <v>305</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>17.8</v>
+        <v>35.9</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>3.2</v>
+        <v>7.9</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>9374</v>
+        <v>7218</v>
       </c>
       <c r="K46" s="1" t="n">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,28 +1784,28 @@
         <v>84</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>138</v>
+        <v>249</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>255886</v>
+        <v>29353</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>180138</v>
+        <v>20421</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>440</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>20.2</v>
+        <v>17.8</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>9655</v>
-      </c>
-      <c r="K47" s="0" t="n">
-        <v>90</v>
+        <v>9374</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,28 +1962,28 @@
         <v>96</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>48</v>
+        <v>155</v>
       </c>
       <c r="D54" s="8" t="n">
-        <v>55872</v>
+        <v>2239</v>
       </c>
       <c r="E54" s="8" t="n">
-        <v>46745</v>
-      </c>
-      <c r="F54" s="1" t="n">
-        <v>440</v>
+        <v>685</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>29.7</v>
+        <v>66.3</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>4.1</v>
+        <v>7.7</v>
       </c>
       <c r="J54" s="1" t="n">
-        <v>9292</v>
+        <v>213</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,28 +2026,28 @@
         <v>100</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>155</v>
+        <v>48</v>
       </c>
       <c r="D56" s="8" t="n">
-        <v>2239</v>
+        <v>55872</v>
       </c>
       <c r="E56" s="8" t="n">
-        <v>685</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>94</v>
+        <v>46745</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>440</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>66.3</v>
+        <v>29.7</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>7.7</v>
+        <v>4.1</v>
       </c>
       <c r="J56" s="1" t="n">
-        <v>213</v>
+        <v>9292</v>
       </c>
       <c r="K56" s="1" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,31 +2093,28 @@
         <v>104</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="D58" s="8" t="n">
-        <v>34532</v>
+        <v>38187</v>
       </c>
       <c r="E58" s="8" t="n">
-        <v>30874</v>
+        <v>29137</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>15</v>
+        <v>310</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>5</v>
+        <v>13.8</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>3.9</v>
+        <v>7.8</v>
       </c>
       <c r="J58" s="8" t="n">
-        <v>9562</v>
+        <v>9056</v>
       </c>
       <c r="K58" s="1" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,28 +2157,31 @@
         <v>108</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="D60" s="8" t="n">
-        <v>38187</v>
+        <v>343083</v>
       </c>
       <c r="E60" s="8" t="n">
-        <v>29137</v>
+        <v>279265</v>
       </c>
       <c r="F60" s="1" t="n">
-        <v>310</v>
+        <v>99</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>13.8</v>
+        <v>1.2</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>7.8</v>
+        <v>3</v>
       </c>
       <c r="J60" s="8" t="n">
-        <v>9056</v>
+        <v>8781</v>
       </c>
       <c r="K60" s="1" t="n">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,31 +2192,31 @@
         <v>110</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="D61" s="8" t="n">
-        <v>343083</v>
+        <v>34532</v>
       </c>
       <c r="E61" s="8" t="n">
-        <v>279265</v>
+        <v>30874</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H61" s="2" t="n">
-        <v>1.2</v>
+        <v>5</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="J61" s="8" t="n">
-        <v>8781</v>
+        <v>9562</v>
       </c>
       <c r="K61" s="1" t="n">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>